<commit_message>
fixed website and committing before including emily's 2024-06-14 slide changes
</commit_message>
<xml_diff>
--- a/case-studies/Tasas-Lesiones-Polvora-Colombia-2007-2022.xlsx
+++ b/case-studies/Tasas-Lesiones-Polvora-Colombia-2007-2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johngraves/Dropbox/teaching/bogota-vital-strategies/case-studies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{213F7458-028A-9449-8FD6-A28E72642105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EBF1D42-15CC-DF4E-9962-8967145268EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8320" yWindow="500" windowWidth="34560" windowHeight="20040" xr2:uid="{9C2694FF-E8A4-4C3C-9EDD-96D00CBC4B22}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20040" xr2:uid="{9C2694FF-E8A4-4C3C-9EDD-96D00CBC4B22}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -356,6 +356,12 @@
     <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -372,12 +378,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -936,21 +936,21 @@
     </row>
     <row r="2" spans="1:13" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="G2" s="37" t="s">
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="G2" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
     </row>
     <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
@@ -966,21 +966,21 @@
       <c r="E3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="41" t="s">
+      <c r="G3" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="36" t="s">
+      <c r="H3" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36" t="s">
+      <c r="I3" s="38"/>
+      <c r="J3" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="K3" s="36"/>
-      <c r="L3" s="37" t="s">
+      <c r="K3" s="38"/>
+      <c r="L3" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="M3" s="37"/>
+      <c r="M3" s="39"/>
     </row>
     <row r="4" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9"/>
@@ -997,7 +997,7 @@
         <f>C4/D4*100000</f>
         <v>0.64465267637521417</v>
       </c>
-      <c r="G4" s="42"/>
+      <c r="G4" s="36"/>
       <c r="H4" s="32" t="s">
         <v>28</v>
       </c>
@@ -1611,12 +1611,12 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
-      <c r="B21" s="38" t="s">
+      <c r="B21" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="38"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="38"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
       <c r="G21" s="11" t="s">
         <v>2</v>
       </c>
@@ -1643,40 +1643,40 @@
       <c r="A22" s="14"/>
       <c r="C22" s="29"/>
       <c r="D22" s="29"/>
-      <c r="G22" s="35" t="s">
+      <c r="G22" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="H22" s="35"/>
-      <c r="I22" s="35"/>
-      <c r="J22" s="35"/>
-      <c r="K22" s="35"/>
-      <c r="L22" s="35"/>
-      <c r="M22" s="35"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="37"/>
+      <c r="L22" s="37"/>
+      <c r="M22" s="37"/>
     </row>
     <row r="23" spans="1:16" ht="20.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
     </row>
     <row r="24" spans="1:16" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
-      <c r="B24" s="37" t="s">
+      <c r="B24" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="37"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="39"/>
       <c r="F24" s="17"/>
-      <c r="G24" s="37" t="s">
+      <c r="G24" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="H24" s="37"/>
-      <c r="I24" s="37"/>
-      <c r="J24" s="37"/>
-      <c r="K24" s="37"/>
-      <c r="L24" s="37"/>
-      <c r="M24" s="37"/>
-      <c r="N24" s="37"/>
-      <c r="O24" s="37"/>
-      <c r="P24" s="37"/>
+      <c r="H24" s="39"/>
+      <c r="I24" s="39"/>
+      <c r="J24" s="39"/>
+      <c r="K24" s="39"/>
+      <c r="L24" s="39"/>
+      <c r="M24" s="39"/>
+      <c r="N24" s="39"/>
+      <c r="O24" s="39"/>
+      <c r="P24" s="39"/>
     </row>
     <row r="25" spans="1:16" s="10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9"/>
@@ -1693,24 +1693,24 @@
         <v>22</v>
       </c>
       <c r="F25" s="18"/>
-      <c r="G25" s="41" t="s">
+      <c r="G25" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="H25" s="36" t="s">
+      <c r="H25" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="I25" s="36"/>
-      <c r="J25" s="36" t="s">
+      <c r="I25" s="38"/>
+      <c r="J25" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="K25" s="36"/>
-      <c r="L25" s="37" t="s">
+      <c r="K25" s="38"/>
+      <c r="L25" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="M25" s="37"/>
-      <c r="N25" s="39"/>
-      <c r="O25" s="37"/>
-      <c r="P25" s="37"/>
+      <c r="M25" s="39"/>
+      <c r="N25" s="41"/>
+      <c r="O25" s="39"/>
+      <c r="P25" s="39"/>
     </row>
     <row r="26" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
@@ -1727,7 +1727,7 @@
         <v>0.75914439626788899</v>
       </c>
       <c r="F26" s="7"/>
-      <c r="G26" s="42"/>
+      <c r="G26" s="36"/>
       <c r="H26" s="32" t="s">
         <v>28</v>
       </c>
@@ -1746,7 +1746,7 @@
       <c r="M26" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="N26" s="40"/>
+      <c r="N26" s="42"/>
       <c r="O26" s="4"/>
       <c r="P26" s="5"/>
     </row>
@@ -2471,12 +2471,12 @@
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
-      <c r="B45" s="38" t="s">
+      <c r="B45" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="C45" s="38"/>
-      <c r="D45" s="38"/>
-      <c r="E45" s="38"/>
+      <c r="C45" s="40"/>
+      <c r="D45" s="40"/>
+      <c r="E45" s="40"/>
       <c r="G45" s="11" t="s">
         <v>2</v>
       </c>
@@ -2504,18 +2504,18 @@
     </row>
     <row r="46" spans="1:16" ht="45.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
-      <c r="G46" s="35" t="s">
+      <c r="G46" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="H46" s="35"/>
-      <c r="I46" s="35"/>
-      <c r="J46" s="35"/>
-      <c r="K46" s="35"/>
-      <c r="L46" s="35"/>
-      <c r="M46" s="35"/>
-      <c r="N46" s="35"/>
-      <c r="O46" s="35"/>
-      <c r="P46" s="35"/>
+      <c r="H46" s="37"/>
+      <c r="I46" s="37"/>
+      <c r="J46" s="37"/>
+      <c r="K46" s="37"/>
+      <c r="L46" s="37"/>
+      <c r="M46" s="37"/>
+      <c r="N46" s="37"/>
+      <c r="O46" s="37"/>
+      <c r="P46" s="37"/>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
@@ -51521,11 +51521,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="G46:P46"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="L25:M25"/>
     <mergeCell ref="B45:E45"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B21:E21"/>
@@ -51539,6 +51534,11 @@
     <mergeCell ref="O25:P25"/>
     <mergeCell ref="N25:N26"/>
     <mergeCell ref="B24:E24"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="G46:P46"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="L25:M25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>